<commit_message>
Full version prior to cleanup
</commit_message>
<xml_diff>
--- a/Parameters_table.xlsx
+++ b/Parameters_table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Model</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>time hrs</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -413,7 +416,7 @@
     <col min="13" max="13" width="10.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,8 +462,11 @@
       <c r="O1" t="s">
         <v>19</v>
       </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -483,7 +489,7 @@
         <v>-0.21</v>
       </c>
       <c r="H2">
-        <v>-8.0999999999999996E-4</v>
+        <v>-8.0000000000000004E-4</v>
       </c>
       <c r="I2">
         <v>49</v>
@@ -506,8 +512,12 @@
       <c r="O2">
         <v>2800</v>
       </c>
+      <c r="P2">
+        <f>O2/3600</f>
+        <v>0.77777777777777779</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -553,26 +563,144 @@
       <c r="O3">
         <v>8045</v>
       </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P6" si="0">O3/3600</f>
+        <v>2.2347222222222221</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>15</v>
       </c>
+      <c r="B4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D4">
+        <v>-8.7999999999999995E-2</v>
+      </c>
+      <c r="E4">
+        <v>74</v>
+      </c>
+      <c r="F4">
+        <v>4.05</v>
+      </c>
+      <c r="G4">
+        <v>-0.21</v>
+      </c>
+      <c r="H4">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+      <c r="I4">
+        <v>49</v>
+      </c>
+      <c r="J4">
+        <v>0.22</v>
+      </c>
+      <c r="K4">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>0.13</v>
+      </c>
+      <c r="M4">
+        <v>77</v>
+      </c>
       <c r="N4">
         <v>750000</v>
       </c>
+      <c r="O4">
+        <v>15600</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>4.333333333333333</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>16</v>
       </c>
+      <c r="F5">
+        <v>3.32</v>
+      </c>
+      <c r="G5">
+        <v>-0.24</v>
+      </c>
+      <c r="H5">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I5">
+        <v>52</v>
+      </c>
+      <c r="J5">
+        <v>0.48</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+      <c r="L5">
+        <v>0.13</v>
+      </c>
+      <c r="M5">
+        <v>86</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+      <c r="D6">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="E6">
+        <v>88</v>
+      </c>
+      <c r="F6">
+        <v>3.32</v>
+      </c>
+      <c r="G6">
+        <v>-0.24</v>
+      </c>
+      <c r="H6">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I6">
+        <v>58</v>
+      </c>
+      <c r="J6">
+        <v>0.08</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>0.04</v>
+      </c>
+      <c r="M6">
+        <v>75</v>
+      </c>
+      <c r="N6">
+        <v>1500000</v>
+      </c>
+      <c r="O6">
+        <v>81300</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>22.583333333333332</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>